<commit_message>
updated and pruned data with sorting
</commit_message>
<xml_diff>
--- a/Companies/Finance - Investment/Bajaj Finserv Ltd/Pruned_Excel/1_Sep13_Sep14.xlsx
+++ b/Companies/Finance - Investment/Bajaj Finserv Ltd/Pruned_Excel/1_Sep13_Sep14.xlsx
@@ -55,13 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,10 +439,6 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="2" customWidth="1" min="7" max="7"/>
-    <col width="7" customWidth="1" min="8" max="8"/>
-    <col width="7" customWidth="1" min="9" max="9"/>
-    <col width="19" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,43 +449,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Sep '13</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Dec '13</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Mar '14</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Jun '14</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Sep '14</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Jun '14</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Mar '14</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Dec '13</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Sep '13</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr"/>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Max</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Min</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Avg</t>
         </is>
       </c>
     </row>
@@ -504,37 +481,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>80.48</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>20.77</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>14.79</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>22.59</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>75.49</t>
         </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>22.59</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>14.79</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>20.77</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>80.48</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>80.48</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>14.79</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>42.824</v>
       </c>
     </row>
     <row r="3">
@@ -545,37 +513,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>80.48</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>20.77</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>14.79</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>22.59</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>75.49</t>
         </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>22.59</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>14.79</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>20.77</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>80.48</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>80.48</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>14.79</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>42.824</v>
       </c>
     </row>
     <row r="4"/>
@@ -594,37 +553,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>3.48</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3.56</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4.34</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>3.80</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>3.76</t>
         </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>3.80</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>4.34</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>3.56</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>3.48</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>4.34</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>3.787999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -635,37 +585,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>0.32</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.32</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>0.72</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>0.72</t>
         </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0.34</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0.32</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0.32</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>0.484</v>
       </c>
     </row>
     <row r="8">
@@ -676,37 +617,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>9.55</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>9.86</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>6.42</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>8.31</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>9.20</t>
         </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>8.31</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>6.42</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>9.86</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>9.55</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>9.859999999999999</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>6.42</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>8.668000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -717,37 +649,28 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>67.13</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>7.03</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3.69</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>9.76</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>61.81</t>
         </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>9.76</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>3.69</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>7.03</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>67.13</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>67.13</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>3.69</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>29.884</v>
       </c>
     </row>
     <row r="10">
@@ -758,37 +681,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>2.80</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3.65</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3.24</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2.95</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>2.73</t>
         </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2.95</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>3.24</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>3.65</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2.80</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>3.65</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>2.73</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>3.074</v>
       </c>
     </row>
     <row r="11">
@@ -799,37 +713,28 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>69.93</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10.68</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6.93</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>12.71</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>64.54</t>
         </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>12.71</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>6.93</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>10.68</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>69.93</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>69.93000000000001</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>6.93</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>32.95800000000001</v>
       </c>
     </row>
     <row r="12">
@@ -840,37 +745,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>69.93</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10.68</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6.93</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>12.71</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>64.54</t>
         </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>12.71</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>6.93</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>10.68</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>69.93</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>69.93000000000001</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>6.93</v>
-      </c>
-      <c r="J12" s="2" t="n">
-        <v>32.95800000000001</v>
       </c>
     </row>
     <row r="13">
@@ -881,37 +777,28 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>-7.24</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>--</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>7.24</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>--</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>7.24</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>--</t>
         </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>-7.24</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>7.24</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>-7.24</v>
-      </c>
-      <c r="J13" s="2" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -922,37 +809,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>62.69</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>10.68</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>14.17</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12.71</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>64.54</t>
         </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>12.71</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>14.17</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>10.68</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>62.69</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>64.54000000000001</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>10.68</v>
-      </c>
-      <c r="J14" s="2" t="n">
-        <v>32.958</v>
       </c>
     </row>
     <row r="15">
@@ -963,37 +841,28 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>6.33</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>5.33</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3.48</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>4.74</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>4.51</t>
         </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>4.74</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>3.48</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>5.33</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>6.33</t>
-        </is>
-      </c>
-      <c r="H15" s="2" t="n">
-        <v>6.33</v>
-      </c>
-      <c r="I15" s="2" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="J15" s="2" t="n">
-        <v>4.878</v>
       </c>
     </row>
     <row r="16">
@@ -1004,37 +873,28 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>56.36</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5.35</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>10.69</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>7.97</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>60.03</t>
         </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>7.97</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>10.69</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>5.35</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>56.36</t>
-        </is>
-      </c>
-      <c r="H16" s="2" t="n">
-        <v>60.03</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <v>5.35</v>
-      </c>
-      <c r="J16" s="2" t="n">
-        <v>28.08</v>
       </c>
     </row>
     <row r="17">
@@ -1068,15 +928,6 @@
           <t>--</t>
         </is>
       </c>
-      <c r="H17" s="2" t="n">
-        <v>-0.12</v>
-      </c>
-      <c r="I17" s="2" t="n">
-        <v>-0.12</v>
-      </c>
-      <c r="J17" s="2" t="n">
-        <v>-0.12</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1086,37 +937,28 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>56.36</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>5.35</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>10.57</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>7.97</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>60.03</t>
         </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>7.97</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>10.57</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>5.35</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>56.36</t>
-        </is>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>60.03</v>
-      </c>
-      <c r="I18" s="2" t="n">
-        <v>5.35</v>
-      </c>
-      <c r="J18" s="2" t="n">
-        <v>28.056</v>
       </c>
     </row>
     <row r="19">
@@ -1149,15 +991,6 @@
         <is>
           <t>79.56</t>
         </is>
-      </c>
-      <c r="H19" s="2" t="n">
-        <v>79.56</v>
-      </c>
-      <c r="I19" s="2" t="n">
-        <v>79.56</v>
-      </c>
-      <c r="J19" s="2" t="n">
-        <v>79.56</v>
       </c>
     </row>
     <row r="20"/>
@@ -1176,37 +1009,28 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>3.50</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
           <t>3.80</t>
         </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>0.50</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>0.70</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>3.50</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="I22" s="2" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="J22" s="2" t="n">
-        <v>1.76</v>
       </c>
     </row>
     <row r="23">
@@ -1217,37 +1041,28 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>3.50</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>3.80</t>
         </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>0.50</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>0.70</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>3.50</t>
-        </is>
-      </c>
-      <c r="H23" s="2" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="I23" s="2" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="J23" s="2" t="n">
-        <v>1.76</v>
       </c>
     </row>
     <row r="24"/>
@@ -1266,37 +1081,28 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>3.50</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
           <t>3.80</t>
         </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>0.50</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>0.70</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>3.50</t>
-        </is>
-      </c>
-      <c r="H26" s="2" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="I26" s="2" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="J26" s="2" t="n">
-        <v>1.76</v>
       </c>
     </row>
     <row r="27">
@@ -1307,37 +1113,28 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>3.50</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
           <t>3.80</t>
         </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>0.50</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>0.70</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>3.50</t>
-        </is>
-      </c>
-      <c r="H27" s="2" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="I27" s="2" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="J27" s="2" t="n">
-        <v>1.76</v>
       </c>
     </row>
     <row r="28"/>
@@ -1379,15 +1176,6 @@
           <t>6.54</t>
         </is>
       </c>
-      <c r="H30" s="2" t="n">
-        <v>6.54</v>
-      </c>
-      <c r="I30" s="2" t="n">
-        <v>6.54</v>
-      </c>
-      <c r="J30" s="2" t="n">
-        <v>6.540000000000001</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1419,15 +1207,6 @@
         <is>
           <t>41.11</t>
         </is>
-      </c>
-      <c r="H31" s="2" t="n">
-        <v>41.11</v>
-      </c>
-      <c r="I31" s="2" t="n">
-        <v>41.11</v>
-      </c>
-      <c r="J31" s="2" t="n">
-        <v>41.11</v>
       </c>
     </row>
     <row r="32"/>
@@ -1485,15 +1264,6 @@
           <t>9.37</t>
         </is>
       </c>
-      <c r="H38" s="2" t="n">
-        <v>9.369999999999999</v>
-      </c>
-      <c r="I38" s="2" t="n">
-        <v>9.369999999999999</v>
-      </c>
-      <c r="J38" s="2" t="n">
-        <v>9.369999999999999</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1526,15 +1296,6 @@
           <t>100.00</t>
         </is>
       </c>
-      <c r="H39" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="I39" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="J39" s="2" t="n">
-        <v>100</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1566,15 +1327,6 @@
         <is>
           <t>58.89</t>
         </is>
-      </c>
-      <c r="H40" s="2" t="n">
-        <v>58.89</v>
-      </c>
-      <c r="I40" s="2" t="n">
-        <v>58.89</v>
-      </c>
-      <c r="J40" s="2" t="n">
-        <v>58.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>